<commit_message>
Upload Y4_B2526_General_Surgery_checklist1758703663545_backup@backdoor.com.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_General_Surgery_checklist1758703663545_backup@backdoor.com.xlsx
+++ b/log_history/Y4_B2526_General_Surgery_checklist1758703663545_backup@backdoor.com.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\log_history\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2864F6-F20E-4EAD-A83A-60F9F3313E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5C3918-6B18-4CC5-BB4A-0BD5644A924F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="1300" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -416,10 +416,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -448,7 +455,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,15 +798,15 @@
   <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D121"/>
+      <selection activeCell="D2" sqref="D2:D121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="24.25" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -819,7 +826,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -830,7 +837,7 @@
         <v>45920</v>
       </c>
       <c r="D2" s="2">
-        <v>0.46875</v>
+        <v>0.46059027777777778</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -839,7 +846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -850,7 +857,7 @@
         <v>45920</v>
       </c>
       <c r="D3" s="2">
-        <v>0.46875</v>
+        <v>0.46059027777777778</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -859,7 +866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -870,7 +877,7 @@
         <v>45920</v>
       </c>
       <c r="D4" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -879,7 +886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -890,7 +897,7 @@
         <v>45920</v>
       </c>
       <c r="D5" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -899,7 +906,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -910,7 +917,7 @@
         <v>45920</v>
       </c>
       <c r="D6" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -919,7 +926,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -930,7 +937,7 @@
         <v>45920</v>
       </c>
       <c r="D7" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -939,7 +946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -950,7 +957,7 @@
         <v>45920</v>
       </c>
       <c r="D8" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
@@ -959,7 +966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -970,7 +977,7 @@
         <v>45920</v>
       </c>
       <c r="D9" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
@@ -979,7 +986,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -990,7 +997,7 @@
         <v>45920</v>
       </c>
       <c r="D10" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
@@ -999,7 +1006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1010,7 +1017,7 @@
         <v>45920</v>
       </c>
       <c r="D11" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
@@ -1019,7 +1026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1030,7 +1037,7 @@
         <v>45920</v>
       </c>
       <c r="D12" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
@@ -1039,7 +1046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1050,7 +1057,7 @@
         <v>45920</v>
       </c>
       <c r="D13" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
@@ -1059,7 +1066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1070,7 +1077,7 @@
         <v>45920</v>
       </c>
       <c r="D14" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E14" t="s">
         <v>13</v>
@@ -1079,7 +1086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1090,7 +1097,7 @@
         <v>45920</v>
       </c>
       <c r="D15" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
@@ -1099,7 +1106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1110,7 +1117,7 @@
         <v>45920</v>
       </c>
       <c r="D16" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E16" t="s">
         <v>13</v>
@@ -1119,7 +1126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1130,7 +1137,7 @@
         <v>45920</v>
       </c>
       <c r="D17" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E17" t="s">
         <v>13</v>
@@ -1139,7 +1146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1150,7 +1157,7 @@
         <v>45920</v>
       </c>
       <c r="D18" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E18" t="s">
         <v>8</v>
@@ -1159,7 +1166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1170,7 +1177,7 @@
         <v>45920</v>
       </c>
       <c r="D19" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E19" t="s">
         <v>13</v>
@@ -1179,7 +1186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1190,7 +1197,7 @@
         <v>45920</v>
       </c>
       <c r="D20" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E20" t="s">
         <v>13</v>
@@ -1199,7 +1206,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1210,7 +1217,7 @@
         <v>45920</v>
       </c>
       <c r="D21" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E21" t="s">
         <v>13</v>
@@ -1219,7 +1226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1230,7 +1237,7 @@
         <v>45920</v>
       </c>
       <c r="D22" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E22" t="s">
         <v>8</v>
@@ -1239,7 +1246,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1250,7 +1257,7 @@
         <v>45920</v>
       </c>
       <c r="D23" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E23" t="s">
         <v>8</v>
@@ -1259,7 +1266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1270,7 +1277,7 @@
         <v>45920</v>
       </c>
       <c r="D24" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E24" t="s">
         <v>13</v>
@@ -1279,7 +1286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1290,7 +1297,7 @@
         <v>45920</v>
       </c>
       <c r="D25" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E25" t="s">
         <v>13</v>
@@ -1299,7 +1306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1310,7 +1317,7 @@
         <v>45920</v>
       </c>
       <c r="D26" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E26" t="s">
         <v>13</v>
@@ -1319,7 +1326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1330,7 +1337,7 @@
         <v>45920</v>
       </c>
       <c r="D27" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E27" t="s">
         <v>13</v>
@@ -1339,7 +1346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1350,7 +1357,7 @@
         <v>45920</v>
       </c>
       <c r="D28" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E28" t="s">
         <v>8</v>
@@ -1359,7 +1366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -1370,7 +1377,7 @@
         <v>45920</v>
       </c>
       <c r="D29" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E29" t="s">
         <v>8</v>
@@ -1379,7 +1386,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -1390,7 +1397,7 @@
         <v>45920</v>
       </c>
       <c r="D30" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E30" t="s">
         <v>13</v>
@@ -1399,7 +1406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -1410,7 +1417,7 @@
         <v>45920</v>
       </c>
       <c r="D31" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E31" t="s">
         <v>13</v>
@@ -1419,7 +1426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -1430,7 +1437,7 @@
         <v>45920</v>
       </c>
       <c r="D32" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E32" t="s">
         <v>13</v>
@@ -1439,7 +1446,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -1450,7 +1457,7 @@
         <v>45920</v>
       </c>
       <c r="D33" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E33" t="s">
         <v>8</v>
@@ -1459,7 +1466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -1470,7 +1477,7 @@
         <v>45920</v>
       </c>
       <c r="D34" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E34" t="s">
         <v>13</v>
@@ -1479,7 +1486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -1490,7 +1497,7 @@
         <v>45920</v>
       </c>
       <c r="D35" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E35" t="s">
         <v>13</v>
@@ -1499,7 +1506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -1510,7 +1517,7 @@
         <v>45920</v>
       </c>
       <c r="D36" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E36" t="s">
         <v>8</v>
@@ -1519,7 +1526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -1530,7 +1537,7 @@
         <v>45920</v>
       </c>
       <c r="D37" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E37" t="s">
         <v>13</v>
@@ -1539,7 +1546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -1550,7 +1557,7 @@
         <v>45920</v>
       </c>
       <c r="D38" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E38" t="s">
         <v>13</v>
@@ -1559,7 +1566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -1570,7 +1577,7 @@
         <v>45920</v>
       </c>
       <c r="D39" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E39" t="s">
         <v>13</v>
@@ -1579,7 +1586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -1590,7 +1597,7 @@
         <v>45920</v>
       </c>
       <c r="D40" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E40" t="s">
         <v>13</v>
@@ -1599,7 +1606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -1610,7 +1617,7 @@
         <v>45920</v>
       </c>
       <c r="D41" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E41" t="s">
         <v>8</v>
@@ -1619,7 +1626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -1630,7 +1637,7 @@
         <v>45920</v>
       </c>
       <c r="D42" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E42" t="s">
         <v>13</v>
@@ -1639,7 +1646,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>51</v>
       </c>
@@ -1650,7 +1657,7 @@
         <v>45920</v>
       </c>
       <c r="D43" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E43" t="s">
         <v>13</v>
@@ -1659,7 +1666,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -1670,7 +1677,7 @@
         <v>45920</v>
       </c>
       <c r="D44" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E44" t="s">
         <v>8</v>
@@ -1679,7 +1686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>53</v>
       </c>
@@ -1690,7 +1697,7 @@
         <v>45920</v>
       </c>
       <c r="D45" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E45" t="s">
         <v>8</v>
@@ -1699,7 +1706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>54</v>
       </c>
@@ -1710,7 +1717,7 @@
         <v>45920</v>
       </c>
       <c r="D46" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E46" t="s">
         <v>8</v>
@@ -1719,7 +1726,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -1730,7 +1737,7 @@
         <v>45920</v>
       </c>
       <c r="D47" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E47" t="s">
         <v>8</v>
@@ -1739,7 +1746,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -1750,7 +1757,7 @@
         <v>45920</v>
       </c>
       <c r="D48" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E48" t="s">
         <v>8</v>
@@ -1759,7 +1766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>57</v>
       </c>
@@ -1770,7 +1777,7 @@
         <v>45920</v>
       </c>
       <c r="D49" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E49" t="s">
         <v>8</v>
@@ -1779,7 +1786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -1790,7 +1797,7 @@
         <v>45920</v>
       </c>
       <c r="D50" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E50" t="s">
         <v>8</v>
@@ -1799,7 +1806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -1810,7 +1817,7 @@
         <v>45920</v>
       </c>
       <c r="D51" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E51" t="s">
         <v>8</v>
@@ -1819,7 +1826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -1830,7 +1837,7 @@
         <v>45920</v>
       </c>
       <c r="D52" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E52" t="s">
         <v>13</v>
@@ -1839,7 +1846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>61</v>
       </c>
@@ -1850,7 +1857,7 @@
         <v>45920</v>
       </c>
       <c r="D53" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E53" t="s">
         <v>13</v>
@@ -1859,7 +1866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>62</v>
       </c>
@@ -1870,7 +1877,7 @@
         <v>45920</v>
       </c>
       <c r="D54" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E54" t="s">
         <v>8</v>
@@ -1879,7 +1886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>63</v>
       </c>
@@ -1890,7 +1897,7 @@
         <v>45920</v>
       </c>
       <c r="D55" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E55" t="s">
         <v>8</v>
@@ -1899,7 +1906,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>64</v>
       </c>
@@ -1910,7 +1917,7 @@
         <v>45920</v>
       </c>
       <c r="D56" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E56" t="s">
         <v>13</v>
@@ -1919,7 +1926,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>65</v>
       </c>
@@ -1930,7 +1937,7 @@
         <v>45920</v>
       </c>
       <c r="D57" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E57" t="s">
         <v>13</v>
@@ -1939,7 +1946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>66</v>
       </c>
@@ -1950,7 +1957,7 @@
         <v>45920</v>
       </c>
       <c r="D58" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E58" t="s">
         <v>13</v>
@@ -1959,7 +1966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>67</v>
       </c>
@@ -1970,7 +1977,7 @@
         <v>45920</v>
       </c>
       <c r="D59" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E59" t="s">
         <v>13</v>
@@ -1979,7 +1986,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -1990,7 +1997,7 @@
         <v>45920</v>
       </c>
       <c r="D60" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E60" t="s">
         <v>13</v>
@@ -1999,7 +2006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>69</v>
       </c>
@@ -2010,7 +2017,7 @@
         <v>45920</v>
       </c>
       <c r="D61" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E61" t="s">
         <v>13</v>
@@ -2019,7 +2026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>70</v>
       </c>
@@ -2030,7 +2037,7 @@
         <v>45920</v>
       </c>
       <c r="D62" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E62" t="s">
         <v>13</v>
@@ -2039,7 +2046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>71</v>
       </c>
@@ -2050,7 +2057,7 @@
         <v>45920</v>
       </c>
       <c r="D63" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E63" t="s">
         <v>13</v>
@@ -2059,7 +2066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>72</v>
       </c>
@@ -2070,7 +2077,7 @@
         <v>45920</v>
       </c>
       <c r="D64" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E64" t="s">
         <v>13</v>
@@ -2079,7 +2086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>73</v>
       </c>
@@ -2090,7 +2097,7 @@
         <v>45920</v>
       </c>
       <c r="D65" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E65" t="s">
         <v>13</v>
@@ -2099,7 +2106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>74</v>
       </c>
@@ -2110,7 +2117,7 @@
         <v>45920</v>
       </c>
       <c r="D66" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E66" t="s">
         <v>13</v>
@@ -2119,7 +2126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>75</v>
       </c>
@@ -2130,7 +2137,7 @@
         <v>45920</v>
       </c>
       <c r="D67" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E67" t="s">
         <v>13</v>
@@ -2139,7 +2146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>76</v>
       </c>
@@ -2150,7 +2157,7 @@
         <v>45920</v>
       </c>
       <c r="D68" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E68" t="s">
         <v>13</v>
@@ -2159,7 +2166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>77</v>
       </c>
@@ -2170,7 +2177,7 @@
         <v>45920</v>
       </c>
       <c r="D69" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E69" t="s">
         <v>13</v>
@@ -2179,7 +2186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>78</v>
       </c>
@@ -2190,7 +2197,7 @@
         <v>45920</v>
       </c>
       <c r="D70" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E70" t="s">
         <v>8</v>
@@ -2199,7 +2206,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>79</v>
       </c>
@@ -2210,7 +2217,7 @@
         <v>45920</v>
       </c>
       <c r="D71" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E71" t="s">
         <v>13</v>
@@ -2219,7 +2226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>80</v>
       </c>
@@ -2230,7 +2237,7 @@
         <v>45920</v>
       </c>
       <c r="D72" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E72" t="s">
         <v>13</v>
@@ -2239,7 +2246,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>81</v>
       </c>
@@ -2250,7 +2257,7 @@
         <v>45920</v>
       </c>
       <c r="D73" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E73" t="s">
         <v>13</v>
@@ -2259,7 +2266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>82</v>
       </c>
@@ -2270,7 +2277,7 @@
         <v>45920</v>
       </c>
       <c r="D74" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E74" t="s">
         <v>13</v>
@@ -2279,7 +2286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>83</v>
       </c>
@@ -2290,7 +2297,7 @@
         <v>45920</v>
       </c>
       <c r="D75" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E75" t="s">
         <v>13</v>
@@ -2299,7 +2306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>84</v>
       </c>
@@ -2310,7 +2317,7 @@
         <v>45920</v>
       </c>
       <c r="D76" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E76" t="s">
         <v>13</v>
@@ -2319,7 +2326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>85</v>
       </c>
@@ -2330,7 +2337,7 @@
         <v>45920</v>
       </c>
       <c r="D77" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E77" t="s">
         <v>13</v>
@@ -2339,7 +2346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>86</v>
       </c>
@@ -2350,7 +2357,7 @@
         <v>45920</v>
       </c>
       <c r="D78" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E78" t="s">
         <v>13</v>
@@ -2359,7 +2366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>87</v>
       </c>
@@ -2370,7 +2377,7 @@
         <v>45920</v>
       </c>
       <c r="D79" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E79" t="s">
         <v>13</v>
@@ -2379,7 +2386,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>88</v>
       </c>
@@ -2390,7 +2397,7 @@
         <v>45920</v>
       </c>
       <c r="D80" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E80" t="s">
         <v>13</v>
@@ -2399,7 +2406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>89</v>
       </c>
@@ -2410,7 +2417,7 @@
         <v>45920</v>
       </c>
       <c r="D81" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E81" t="s">
         <v>13</v>
@@ -2419,7 +2426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>90</v>
       </c>
@@ -2430,7 +2437,7 @@
         <v>45920</v>
       </c>
       <c r="D82" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E82" t="s">
         <v>13</v>
@@ -2439,7 +2446,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>91</v>
       </c>
@@ -2450,7 +2457,7 @@
         <v>45920</v>
       </c>
       <c r="D83" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E83" t="s">
         <v>13</v>
@@ -2459,7 +2466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>92</v>
       </c>
@@ -2470,7 +2477,7 @@
         <v>45920</v>
       </c>
       <c r="D84" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E84" t="s">
         <v>13</v>
@@ -2479,7 +2486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>93</v>
       </c>
@@ -2490,7 +2497,7 @@
         <v>45920</v>
       </c>
       <c r="D85" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E85" t="s">
         <v>13</v>
@@ -2499,7 +2506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>94</v>
       </c>
@@ -2510,7 +2517,7 @@
         <v>45920</v>
       </c>
       <c r="D86" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E86" t="s">
         <v>13</v>
@@ -2519,7 +2526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>95</v>
       </c>
@@ -2530,7 +2537,7 @@
         <v>45920</v>
       </c>
       <c r="D87" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E87" t="s">
         <v>13</v>
@@ -2539,7 +2546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>96</v>
       </c>
@@ -2550,7 +2557,7 @@
         <v>45920</v>
       </c>
       <c r="D88" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E88" t="s">
         <v>13</v>
@@ -2559,7 +2566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>97</v>
       </c>
@@ -2570,7 +2577,7 @@
         <v>45920</v>
       </c>
       <c r="D89" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E89" t="s">
         <v>8</v>
@@ -2579,7 +2586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>98</v>
       </c>
@@ -2590,7 +2597,7 @@
         <v>45920</v>
       </c>
       <c r="D90" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E90" t="s">
         <v>13</v>
@@ -2599,7 +2606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>99</v>
       </c>
@@ -2610,7 +2617,7 @@
         <v>45920</v>
       </c>
       <c r="D91" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E91" t="s">
         <v>13</v>
@@ -2619,7 +2626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>100</v>
       </c>
@@ -2630,7 +2637,7 @@
         <v>45920</v>
       </c>
       <c r="D92" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E92" t="s">
         <v>13</v>
@@ -2639,7 +2646,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>101</v>
       </c>
@@ -2650,7 +2657,7 @@
         <v>45920</v>
       </c>
       <c r="D93" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E93" t="s">
         <v>13</v>
@@ -2659,7 +2666,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>102</v>
       </c>
@@ -2670,7 +2677,7 @@
         <v>45920</v>
       </c>
       <c r="D94" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E94" t="s">
         <v>13</v>
@@ -2679,7 +2686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>103</v>
       </c>
@@ -2690,7 +2697,7 @@
         <v>45920</v>
       </c>
       <c r="D95" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E95" t="s">
         <v>13</v>
@@ -2699,7 +2706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>104</v>
       </c>
@@ -2710,7 +2717,7 @@
         <v>45920</v>
       </c>
       <c r="D96" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E96" t="s">
         <v>13</v>
@@ -2719,7 +2726,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>105</v>
       </c>
@@ -2730,7 +2737,7 @@
         <v>45920</v>
       </c>
       <c r="D97" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E97" t="s">
         <v>13</v>
@@ -2739,7 +2746,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>106</v>
       </c>
@@ -2750,7 +2757,7 @@
         <v>45920</v>
       </c>
       <c r="D98" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E98" t="s">
         <v>13</v>
@@ -2759,7 +2766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>107</v>
       </c>
@@ -2770,7 +2777,7 @@
         <v>45920</v>
       </c>
       <c r="D99" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E99" t="s">
         <v>13</v>
@@ -2779,7 +2786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>108</v>
       </c>
@@ -2790,7 +2797,7 @@
         <v>45920</v>
       </c>
       <c r="D100" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E100" t="s">
         <v>13</v>
@@ -2799,7 +2806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>109</v>
       </c>
@@ -2810,7 +2817,7 @@
         <v>45920</v>
       </c>
       <c r="D101" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E101" t="s">
         <v>13</v>
@@ -2819,7 +2826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>110</v>
       </c>
@@ -2830,7 +2837,7 @@
         <v>45920</v>
       </c>
       <c r="D102" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E102" t="s">
         <v>13</v>
@@ -2839,7 +2846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>111</v>
       </c>
@@ -2850,7 +2857,7 @@
         <v>45920</v>
       </c>
       <c r="D103" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E103" t="s">
         <v>13</v>
@@ -2859,7 +2866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>112</v>
       </c>
@@ -2870,7 +2877,7 @@
         <v>45920</v>
       </c>
       <c r="D104" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E104" t="s">
         <v>13</v>
@@ -2879,7 +2886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>113</v>
       </c>
@@ -2890,7 +2897,7 @@
         <v>45920</v>
       </c>
       <c r="D105" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E105" t="s">
         <v>13</v>
@@ -2899,7 +2906,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>114</v>
       </c>
@@ -2910,7 +2917,7 @@
         <v>45920</v>
       </c>
       <c r="D106" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E106" t="s">
         <v>13</v>
@@ -2919,7 +2926,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>115</v>
       </c>
@@ -2930,7 +2937,7 @@
         <v>45920</v>
       </c>
       <c r="D107" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E107" t="s">
         <v>13</v>
@@ -2939,7 +2946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>116</v>
       </c>
@@ -2950,7 +2957,7 @@
         <v>45920</v>
       </c>
       <c r="D108" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E108" t="s">
         <v>13</v>
@@ -2959,7 +2966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>117</v>
       </c>
@@ -2970,7 +2977,7 @@
         <v>45920</v>
       </c>
       <c r="D109" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E109" t="s">
         <v>13</v>
@@ -2979,7 +2986,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>118</v>
       </c>
@@ -2990,7 +2997,7 @@
         <v>45920</v>
       </c>
       <c r="D110" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E110" t="s">
         <v>13</v>
@@ -2999,7 +3006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>119</v>
       </c>
@@ -3010,7 +3017,7 @@
         <v>45920</v>
       </c>
       <c r="D111" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E111" t="s">
         <v>13</v>
@@ -3019,7 +3026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>120</v>
       </c>
@@ -3030,7 +3037,7 @@
         <v>45920</v>
       </c>
       <c r="D112" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E112" t="s">
         <v>13</v>
@@ -3039,7 +3046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>121</v>
       </c>
@@ -3050,7 +3057,7 @@
         <v>45920</v>
       </c>
       <c r="D113" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E113" t="s">
         <v>13</v>
@@ -3059,7 +3066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>122</v>
       </c>
@@ -3070,7 +3077,7 @@
         <v>45920</v>
       </c>
       <c r="D114" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E114" t="s">
         <v>13</v>
@@ -3079,7 +3086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>123</v>
       </c>
@@ -3090,7 +3097,7 @@
         <v>45920</v>
       </c>
       <c r="D115" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E115" t="s">
         <v>13</v>
@@ -3099,7 +3106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>124</v>
       </c>
@@ -3110,7 +3117,7 @@
         <v>45920</v>
       </c>
       <c r="D116" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E116" t="s">
         <v>13</v>
@@ -3119,7 +3126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>125</v>
       </c>
@@ -3130,7 +3137,7 @@
         <v>45920</v>
       </c>
       <c r="D117" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E117" t="s">
         <v>13</v>
@@ -3139,7 +3146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>126</v>
       </c>
@@ -3150,7 +3157,7 @@
         <v>45920</v>
       </c>
       <c r="D118" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E118" t="s">
         <v>13</v>
@@ -3159,7 +3166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>127</v>
       </c>
@@ -3170,7 +3177,7 @@
         <v>45920</v>
       </c>
       <c r="D119" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E119" t="s">
         <v>8</v>
@@ -3179,7 +3186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>128</v>
       </c>
@@ -3190,7 +3197,7 @@
         <v>45920</v>
       </c>
       <c r="D120" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E120" t="s">
         <v>8</v>
@@ -3199,7 +3206,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>129</v>
       </c>
@@ -3210,7 +3217,7 @@
         <v>45920</v>
       </c>
       <c r="D121" s="2">
-        <v>0.46875</v>
+        <v>0.460590277777778</v>
       </c>
       <c r="E121" t="s">
         <v>8</v>

</xml_diff>